<commit_message>
Updates based on IA revisions and tree test 2 approach
Former-commit-id: a66cb194e786aafeec3c9db57555e9a18ba10b58
</commit_message>
<xml_diff>
--- a/design/content/VA.gov-Nav-Hub-Links_wip.xlsx
+++ b/design/content/VA.gov-Nav-Hub-Links_wip.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2080" uniqueCount="798">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2080" uniqueCount="800">
   <si>
     <t>Inside VA</t>
   </si>
@@ -2645,45 +2645,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Notes: 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>6/27 - Revised top nav to max of 5 links as well as ongoing updates
-6/13 - Revisions based on VHA feedback</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>6/6 - Revisions based on VHA feedback</t>
-    </r>
-  </si>
-  <si>
     <t>How to Apply</t>
   </si>
   <si>
@@ -3134,45 +3095,6 @@
     <t>More VA Benefits and Services</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Notes: 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>6/28 - Updated post content audit and tree test findings
-6/13 - Revisions based on NCA feedback</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>6/6 - Revisions based on NCA and IA feedback</t>
-    </r>
-  </si>
-  <si>
     <t>About Burial and Memorial Benefits</t>
   </si>
   <si>
@@ -3241,10 +3163,6 @@
   </si>
   <si>
     <t>Get Your Records and Documents</t>
-  </si>
-  <si>
-    <t>Notes: 
-6/28-Updated based on new top nav limitations of 5 links per column</t>
   </si>
   <si>
     <t>Apply Now for Health Care</t>
@@ -3403,6 +3321,167 @@
   </si>
   <si>
     <t xml:space="preserve">Apply Now for a SAH Grant </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Notes: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>7/11 -Updates based on IA revisions and tree test 2 approach</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>6/28 - Updated post content audit and tree test findings</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Notes: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>7/11 -Updates based on IA revisions and tree test 2 approach</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>6/27 - Revised top nav to max of 5 links as well as ongoing updates
+6/13 - Revisions based on VHA feedback</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>6/6 - Revisions based on VHA feedback</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Notes: 
+7/11 -Updates based on IA revisions and tree test 2 approach
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>6/28 - Updated post content audit and tree test findings</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Notes: 
+7/11 -Updates based on IA revisions and tree test 2 approach
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>6/28 - Updated post content audit and tree test findings
+6/13 - Revisions based on NCA feedback</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>6/6 - Revisions based on NCA and IA feedback</t>
+    </r>
+  </si>
+  <si>
+    <t>Notes: 
+7/11 -Updates based on IA revisions and tree test 2 approach
+6/28-Updated based on new top nav limitations of 5 links per column</t>
   </si>
 </sst>
 </file>
@@ -4146,14 +4225,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -4760,8 +4839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -4796,11 +4875,11 @@
       <c r="B2" s="25">
         <v>43292</v>
       </c>
-      <c r="C2" s="156" t="s">
-        <v>766</v>
-      </c>
-      <c r="D2" s="156"/>
-      <c r="E2" s="156"/>
+      <c r="C2" s="157" t="s">
+        <v>799</v>
+      </c>
+      <c r="D2" s="157"/>
+      <c r="E2" s="157"/>
       <c r="G2" s="41" t="s">
         <v>195</v>
       </c>
@@ -4810,9 +4889,9 @@
         <v>46</v>
       </c>
       <c r="B3" s="145"/>
-      <c r="C3" s="156"/>
-      <c r="D3" s="156"/>
-      <c r="E3" s="156"/>
+      <c r="C3" s="157"/>
+      <c r="D3" s="157"/>
+      <c r="E3" s="157"/>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="10" t="s">
@@ -4821,16 +4900,16 @@
       <c r="B4" s="129" t="s">
         <v>345</v>
       </c>
-      <c r="C4" s="156"/>
-      <c r="D4" s="156"/>
-      <c r="E4" s="156"/>
+      <c r="C4" s="157"/>
+      <c r="D4" s="157"/>
+      <c r="E4" s="157"/>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="20"/>
       <c r="B5" s="145"/>
-      <c r="C5" s="156"/>
-      <c r="D5" s="156"/>
-      <c r="E5" s="156"/>
+      <c r="C5" s="157"/>
+      <c r="D5" s="157"/>
+      <c r="E5" s="157"/>
     </row>
     <row r="6" spans="1:12" s="9" customFormat="1" ht="47.25">
       <c r="A6" s="39" t="s">
@@ -4893,7 +4972,7 @@
         <v>198</v>
       </c>
       <c r="B9" s="48" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="C9" s="81" t="s">
         <v>189</v>
@@ -4985,7 +5064,7 @@
         <v>199</v>
       </c>
       <c r="B13" s="124" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="C13" s="129" t="s">
         <v>353</v>
@@ -5021,7 +5100,7 @@
         <v>198</v>
       </c>
       <c r="B15" s="48" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="C15" s="81" t="s">
         <v>189</v>
@@ -5036,7 +5115,7 @@
         <v>298</v>
       </c>
       <c r="G15" s="36" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="H15" s="58"/>
       <c r="I15" s="77"/>
@@ -7472,8 +7551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -7505,10 +7584,10 @@
         <v>45</v>
       </c>
       <c r="B2" s="31">
-        <v>43279</v>
+        <v>43292</v>
       </c>
       <c r="C2" s="154" t="s">
-        <v>656</v>
+        <v>796</v>
       </c>
       <c r="D2" s="154"/>
       <c r="E2" s="154"/>
@@ -7677,7 +7756,7 @@
         <v>199</v>
       </c>
       <c r="B14" s="59" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="C14" s="59" t="s">
         <v>202</v>
@@ -7690,7 +7769,7 @@
         <v>3</v>
       </c>
       <c r="G14" s="43" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="31.5">
@@ -7698,7 +7777,7 @@
         <v>199</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="C15" s="59" t="s">
         <v>205</v>
@@ -7827,7 +7906,7 @@
         <v>199</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="C23" s="59" t="s">
         <v>245</v>
@@ -7845,7 +7924,7 @@
         <v>199</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="C24" s="59" t="s">
         <v>244</v>
@@ -7863,7 +7942,7 @@
         <v>199</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="C25" s="59" t="s">
         <v>243</v>
@@ -7881,7 +7960,7 @@
         <v>199</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="C26" s="59" t="s">
         <v>206</v>
@@ -7983,7 +8062,7 @@
         <v>199</v>
       </c>
       <c r="B31" s="130" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="C31" s="59" t="s">
         <v>401</v>
@@ -7995,7 +8074,7 @@
         <v>9</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="31.5">
@@ -8182,7 +8261,7 @@
         <v>199</v>
       </c>
       <c r="B41" s="64" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C41" s="59" t="s">
         <v>219</v>
@@ -8194,7 +8273,7 @@
         <v>4</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="H41" s="44" t="s">
         <v>607</v>
@@ -8217,7 +8296,7 @@
         <v>5</v>
       </c>
       <c r="G42" s="43" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="H42" s="44" t="s">
         <v>609</v>
@@ -8257,7 +8336,7 @@
         <v>7</v>
       </c>
       <c r="G44" s="43" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -8294,7 +8373,7 @@
         <v>9</v>
       </c>
       <c r="G46" s="43" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="31.5">
@@ -8310,7 +8389,7 @@
         <v>10</v>
       </c>
       <c r="G47" s="44" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="31.5">
@@ -8324,7 +8403,7 @@
       <c r="E48" s="43"/>
       <c r="F48" s="130"/>
       <c r="G48" s="44" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="H48" s="43" t="s">
         <v>610</v>
@@ -8335,7 +8414,7 @@
         <v>229</v>
       </c>
       <c r="B49" s="49" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C49" s="53" t="s">
         <v>189</v>
@@ -8597,8 +8676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K98"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -8630,13 +8709,13 @@
         <v>45</v>
       </c>
       <c r="B2" s="25">
-        <v>43279</v>
-      </c>
-      <c r="C2" s="156" t="s">
-        <v>683</v>
-      </c>
-      <c r="D2" s="157"/>
-      <c r="E2" s="157"/>
+        <v>43292</v>
+      </c>
+      <c r="C2" s="157" t="s">
+        <v>795</v>
+      </c>
+      <c r="D2" s="158"/>
+      <c r="E2" s="158"/>
       <c r="G2" s="41" t="s">
         <v>195</v>
       </c>
@@ -8646,9 +8725,9 @@
         <v>46</v>
       </c>
       <c r="B3" s="87"/>
-      <c r="C3" s="157"/>
-      <c r="D3" s="157"/>
-      <c r="E3" s="157"/>
+      <c r="C3" s="158"/>
+      <c r="D3" s="158"/>
+      <c r="E3" s="158"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="88" t="s">
@@ -8657,16 +8736,16 @@
       <c r="B4" s="87" t="s">
         <v>367</v>
       </c>
-      <c r="C4" s="157"/>
-      <c r="D4" s="157"/>
-      <c r="E4" s="157"/>
+      <c r="C4" s="158"/>
+      <c r="D4" s="158"/>
+      <c r="E4" s="158"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="87"/>
       <c r="B5" s="87"/>
-      <c r="C5" s="157"/>
-      <c r="D5" s="157"/>
-      <c r="E5" s="157"/>
+      <c r="C5" s="158"/>
+      <c r="D5" s="158"/>
+      <c r="E5" s="158"/>
     </row>
     <row r="6" spans="1:11" s="9" customFormat="1" ht="47.25">
       <c r="A6" s="39" t="s">
@@ -8688,7 +8767,7 @@
         <v>240</v>
       </c>
       <c r="G6" s="40" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="H6" s="40" t="s">
         <v>318</v>
@@ -8780,7 +8859,7 @@
         <v>199</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="C11" s="45" t="s">
         <v>477</v>
@@ -8792,7 +8871,7 @@
         <v>2</v>
       </c>
       <c r="G11" s="43" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="H11" s="58"/>
       <c r="I11" s="58"/>
@@ -8804,7 +8883,7 @@
         <v>199</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="C12" s="45" t="s">
         <v>479</v>
@@ -8963,7 +9042,7 @@
       </c>
       <c r="F20" s="155"/>
       <c r="G20" s="58" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="H20" s="58"/>
       <c r="I20" s="58"/>
@@ -9028,7 +9107,7 @@
         <v>199</v>
       </c>
       <c r="B24" s="130" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="E24" s="59">
         <v>2</v>
@@ -9079,7 +9158,7 @@
         <v>199</v>
       </c>
       <c r="B27" s="100" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="E27" s="59">
         <v>5</v>
@@ -9096,7 +9175,7 @@
         <v>199</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="C28" s="45" t="s">
         <v>361</v>
@@ -9113,7 +9192,7 @@
         <v>199</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
       <c r="C29" s="90" t="s">
         <v>363</v>
@@ -9142,7 +9221,7 @@
         <v>8</v>
       </c>
       <c r="G30" s="100" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="31" spans="1:11" s="100" customFormat="1" ht="47.25">
@@ -9150,7 +9229,7 @@
         <v>199</v>
       </c>
       <c r="B31" s="77" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
       <c r="C31" s="90" t="s">
         <v>480</v>
@@ -9162,7 +9241,7 @@
         <v>9</v>
       </c>
       <c r="G31" s="108" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="H31" s="100" t="s">
         <v>404</v>
@@ -9199,7 +9278,7 @@
       </c>
       <c r="F33" s="155"/>
       <c r="G33" s="7" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="H33" s="108" t="s">
         <v>378</v>
@@ -9242,7 +9321,7 @@
         <v>199</v>
       </c>
       <c r="B36" s="130" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C36" s="45" t="s">
         <v>483</v>
@@ -9254,7 +9333,7 @@
         <v>1</v>
       </c>
       <c r="G36" s="44" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="43" customFormat="1" ht="31.5">
@@ -9299,7 +9378,7 @@
         <v>486</v>
       </c>
       <c r="C39" s="128" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>189</v>
@@ -9308,7 +9387,7 @@
         <v>4</v>
       </c>
       <c r="G39" s="44" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="43" customFormat="1" ht="31.5">
@@ -9328,7 +9407,7 @@
         <v>5</v>
       </c>
       <c r="G40" s="100" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="H40" s="44" t="s">
         <v>580</v>
@@ -9351,7 +9430,7 @@
         <v>6</v>
       </c>
       <c r="G41" s="43" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="H41" s="108" t="s">
         <v>578</v>
@@ -9409,12 +9488,12 @@
       <c r="C46" s="146" t="s">
         <v>653</v>
       </c>
-      <c r="E46" s="158" t="s">
+      <c r="E46" s="156" t="s">
         <v>262</v>
       </c>
-      <c r="F46" s="158"/>
+      <c r="F46" s="156"/>
       <c r="G46" s="7" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="H46" s="43" t="s">
         <v>404</v>
@@ -9428,10 +9507,10 @@
       <c r="C47" s="146" t="s">
         <v>489</v>
       </c>
-      <c r="E47" s="158" t="s">
+      <c r="E47" s="156" t="s">
         <v>262</v>
       </c>
-      <c r="F47" s="158"/>
+      <c r="F47" s="156"/>
       <c r="G47" s="43" t="s">
         <v>652</v>
       </c>
@@ -9444,10 +9523,10 @@
       <c r="C48" s="146" t="s">
         <v>495</v>
       </c>
-      <c r="E48" s="158" t="s">
+      <c r="E48" s="156" t="s">
         <v>262</v>
       </c>
-      <c r="F48" s="158"/>
+      <c r="F48" s="156"/>
       <c r="G48" s="43" t="s">
         <v>652</v>
       </c>
@@ -9463,12 +9542,12 @@
       <c r="C49" s="146" t="s">
         <v>493</v>
       </c>
-      <c r="E49" s="158" t="s">
+      <c r="E49" s="156" t="s">
         <v>262</v>
       </c>
-      <c r="F49" s="158"/>
+      <c r="F49" s="156"/>
       <c r="G49" s="119" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="H49" s="44" t="s">
         <v>579</v>
@@ -9482,12 +9561,12 @@
       <c r="C50" s="146" t="s">
         <v>488</v>
       </c>
-      <c r="E50" s="158" t="s">
+      <c r="E50" s="156" t="s">
         <v>262</v>
       </c>
-      <c r="F50" s="158"/>
+      <c r="F50" s="156"/>
       <c r="G50" s="7" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="H50" s="43" t="s">
         <v>404</v>
@@ -9501,12 +9580,12 @@
       <c r="C51" s="146" t="s">
         <v>497</v>
       </c>
-      <c r="E51" s="158" t="s">
+      <c r="E51" s="156" t="s">
         <v>262</v>
       </c>
-      <c r="F51" s="158"/>
+      <c r="F51" s="156"/>
       <c r="G51" s="7" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="H51" s="43" t="s">
         <v>404</v>
@@ -9517,7 +9596,7 @@
         <v>229</v>
       </c>
       <c r="B52" s="49" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="C52" s="53" t="s">
         <v>189</v>
@@ -9582,7 +9661,7 @@
         <v>507</v>
       </c>
       <c r="C55" s="94" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="E55" s="43" t="s">
         <v>189</v>
@@ -9591,7 +9670,7 @@
         <v>3</v>
       </c>
       <c r="G55" s="44" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="H55" s="43" t="s">
         <v>404</v>
@@ -9644,12 +9723,12 @@
       <c r="C58" s="146" t="s">
         <v>504</v>
       </c>
-      <c r="E58" s="158" t="s">
+      <c r="E58" s="156" t="s">
         <v>262</v>
       </c>
-      <c r="F58" s="158"/>
+      <c r="F58" s="156"/>
       <c r="G58" s="100" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="H58" s="43" t="s">
         <v>404</v>
@@ -9665,12 +9744,12 @@
       <c r="C59" s="146" t="s">
         <v>506</v>
       </c>
-      <c r="E59" s="158" t="s">
+      <c r="E59" s="156" t="s">
         <v>262</v>
       </c>
-      <c r="F59" s="158"/>
+      <c r="F59" s="156"/>
       <c r="G59" s="100" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="H59" s="43" t="s">
         <v>404</v>
@@ -9686,12 +9765,12 @@
       <c r="C60" s="146" t="s">
         <v>392</v>
       </c>
-      <c r="E60" s="158" t="s">
+      <c r="E60" s="156" t="s">
         <v>262</v>
       </c>
-      <c r="F60" s="158"/>
+      <c r="F60" s="156"/>
       <c r="G60" s="119" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="H60" s="108" t="s">
         <v>576</v>
@@ -9707,12 +9786,12 @@
       <c r="C61" s="146" t="s">
         <v>394</v>
       </c>
-      <c r="E61" s="158" t="s">
+      <c r="E61" s="156" t="s">
         <v>262</v>
       </c>
-      <c r="F61" s="158"/>
+      <c r="F61" s="156"/>
       <c r="G61" s="119" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="H61" s="108" t="s">
         <v>577</v>
@@ -9728,12 +9807,12 @@
       <c r="C62" s="146" t="s">
         <v>54</v>
       </c>
-      <c r="E62" s="158" t="s">
+      <c r="E62" s="156" t="s">
         <v>262</v>
       </c>
-      <c r="F62" s="158"/>
+      <c r="F62" s="156"/>
       <c r="G62" s="7" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="63" spans="1:9" s="100" customFormat="1">
@@ -9918,11 +9997,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="E58:F58"/>
-    <mergeCell ref="E59:F59"/>
-    <mergeCell ref="E60:F60"/>
-    <mergeCell ref="E61:F61"/>
     <mergeCell ref="C2:E5"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="E33:F33"/>
@@ -9932,6 +10006,11 @@
     <mergeCell ref="E48:F48"/>
     <mergeCell ref="E49:F49"/>
     <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="E60:F60"/>
+    <mergeCell ref="E61:F61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9941,8 +10020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K98"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -9973,13 +10052,13 @@
         <v>45</v>
       </c>
       <c r="B2" s="25">
-        <v>43279</v>
-      </c>
-      <c r="C2" s="156" t="s">
-        <v>683</v>
-      </c>
-      <c r="D2" s="157"/>
-      <c r="E2" s="157"/>
+        <v>43292</v>
+      </c>
+      <c r="C2" s="157" t="s">
+        <v>797</v>
+      </c>
+      <c r="D2" s="158"/>
+      <c r="E2" s="158"/>
       <c r="G2" s="41" t="s">
         <v>195</v>
       </c>
@@ -9989,9 +10068,9 @@
         <v>46</v>
       </c>
       <c r="B3" s="20"/>
-      <c r="C3" s="157"/>
-      <c r="D3" s="157"/>
-      <c r="E3" s="157"/>
+      <c r="C3" s="158"/>
+      <c r="D3" s="158"/>
+      <c r="E3" s="158"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="10" t="s">
@@ -10000,16 +10079,16 @@
       <c r="B4" s="20" t="s">
         <v>367</v>
       </c>
-      <c r="C4" s="157"/>
-      <c r="D4" s="157"/>
-      <c r="E4" s="157"/>
+      <c r="C4" s="158"/>
+      <c r="D4" s="158"/>
+      <c r="E4" s="158"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="20"/>
       <c r="B5" s="20"/>
-      <c r="C5" s="157"/>
-      <c r="D5" s="157"/>
-      <c r="E5" s="157"/>
+      <c r="C5" s="158"/>
+      <c r="D5" s="158"/>
+      <c r="E5" s="158"/>
     </row>
     <row r="6" spans="1:11" s="9" customFormat="1" ht="47.25">
       <c r="A6" s="39" t="s">
@@ -10140,7 +10219,7 @@
         <v>199</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="C12" s="45" t="s">
         <v>512</v>
@@ -10152,7 +10231,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="43" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="H12" s="58"/>
       <c r="I12" s="58"/>
@@ -10162,7 +10241,7 @@
     <row r="13" spans="1:11" s="68" customFormat="1" ht="31.5">
       <c r="A13" s="131"/>
       <c r="B13" s="130" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
       <c r="C13" s="45" t="s">
         <v>512</v>
@@ -10174,7 +10253,7 @@
         <v>8</v>
       </c>
       <c r="G13" s="58" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="H13" s="58"/>
       <c r="I13" s="58"/>
@@ -10220,7 +10299,7 @@
         <v>5</v>
       </c>
       <c r="G15" s="58" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="H15" s="58"/>
       <c r="I15" s="58"/>
@@ -10235,7 +10314,7 @@
         <v>635</v>
       </c>
       <c r="C16" s="146" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="E16" s="59">
         <v>4</v>
@@ -10244,7 +10323,7 @@
         <v>6</v>
       </c>
       <c r="G16" s="58" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="H16" s="58"/>
       <c r="I16" s="58"/>
@@ -10397,7 +10476,7 @@
         <v>199</v>
       </c>
       <c r="B25" s="130" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C25" s="130" t="s">
         <v>512</v>
@@ -10409,7 +10488,7 @@
         <v>4</v>
       </c>
       <c r="G25" s="97" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="26" spans="1:11" s="100" customFormat="1">
@@ -10427,7 +10506,7 @@
         <v>5</v>
       </c>
       <c r="G26" s="100" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="27" spans="1:11" s="28" customFormat="1" ht="63">
@@ -10438,7 +10517,7 @@
         <v>520</v>
       </c>
       <c r="C27" s="147" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="E27" s="59" t="s">
         <v>212</v>
@@ -10447,7 +10526,7 @@
         <v>6</v>
       </c>
       <c r="G27" s="108" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="28" customFormat="1">
@@ -10465,7 +10544,7 @@
         <v>7</v>
       </c>
       <c r="G28" s="28" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="29" spans="1:11" s="28" customFormat="1" ht="31.5">
@@ -10473,10 +10552,10 @@
         <v>199</v>
       </c>
       <c r="B29" s="130" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="C29" s="130" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="E29" s="59" t="s">
         <v>212</v>
@@ -10485,7 +10564,7 @@
         <v>8</v>
       </c>
       <c r="G29" s="28" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="30" spans="1:11" s="28" customFormat="1" ht="31.5">
@@ -10493,10 +10572,10 @@
         <v>199</v>
       </c>
       <c r="B30" s="130" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C30" s="130" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="E30" s="43" t="s">
         <v>212</v>
@@ -10505,7 +10584,7 @@
         <v>9</v>
       </c>
       <c r="G30" s="28" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="31" spans="1:11" s="28" customFormat="1">
@@ -10532,7 +10611,7 @@
       <c r="E32" s="43"/>
       <c r="F32" s="59"/>
       <c r="G32" s="7" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="H32" s="92" t="s">
         <v>378</v>
@@ -10586,7 +10665,7 @@
         <v>199</v>
       </c>
       <c r="B35" s="77" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C35" s="94" t="s">
         <v>524</v>
@@ -10599,7 +10678,7 @@
         <v>2</v>
       </c>
       <c r="G35" s="44" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="H35" s="44" t="s">
         <v>536</v>
@@ -10610,10 +10689,10 @@
         <v>199</v>
       </c>
       <c r="B36" s="77" t="s">
+        <v>705</v>
+      </c>
+      <c r="C36" s="135" t="s">
         <v>706</v>
-      </c>
-      <c r="C36" s="135" t="s">
-        <v>707</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>189</v>
@@ -10654,7 +10733,7 @@
         <v>5</v>
       </c>
       <c r="G38" s="43" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="43" customFormat="1">
@@ -10671,7 +10750,7 @@
         <v>6</v>
       </c>
       <c r="G39" s="43" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="43" customFormat="1" ht="31.5">
@@ -10679,7 +10758,7 @@
         <v>199</v>
       </c>
       <c r="B40" s="43" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="C40" s="59"/>
       <c r="E40" s="7" t="s">
@@ -10689,7 +10768,7 @@
         <v>7</v>
       </c>
       <c r="G40" s="44" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="43" customFormat="1" ht="31.5">
@@ -10738,17 +10817,17 @@
     <row r="44" spans="1:9" s="43" customFormat="1" ht="31.5">
       <c r="A44" s="131"/>
       <c r="B44" s="146" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="C44" s="146" t="s">
         <v>527</v>
       </c>
-      <c r="E44" s="158" t="s">
+      <c r="E44" s="156" t="s">
         <v>262</v>
       </c>
-      <c r="F44" s="158"/>
+      <c r="F44" s="156"/>
       <c r="G44" s="43" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="45" spans="1:9" s="43" customFormat="1" ht="31.5">
@@ -10759,12 +10838,12 @@
       <c r="C45" s="146" t="s">
         <v>525</v>
       </c>
-      <c r="E45" s="158" t="s">
+      <c r="E45" s="156" t="s">
         <v>262</v>
       </c>
-      <c r="F45" s="158"/>
+      <c r="F45" s="156"/>
       <c r="G45" s="130" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="H45" s="44" t="s">
         <v>537</v>
@@ -10775,7 +10854,7 @@
         <v>229</v>
       </c>
       <c r="B46" s="49" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C46" s="53" t="s">
         <v>189</v>
@@ -10812,7 +10891,7 @@
         <v>1</v>
       </c>
       <c r="G47" s="44" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="H47" s="103" t="s">
         <v>422</v>
@@ -10894,12 +10973,12 @@
       <c r="C52" s="146" t="s">
         <v>529</v>
       </c>
-      <c r="E52" s="158" t="s">
+      <c r="E52" s="156" t="s">
         <v>262</v>
       </c>
-      <c r="F52" s="158"/>
+      <c r="F52" s="156"/>
       <c r="G52" s="44" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="H52" s="43" t="s">
         <v>534</v>
@@ -10913,12 +10992,12 @@
       <c r="C53" s="146" t="s">
         <v>531</v>
       </c>
-      <c r="E53" s="158" t="s">
+      <c r="E53" s="156" t="s">
         <v>262</v>
       </c>
-      <c r="F53" s="158"/>
+      <c r="F53" s="156"/>
       <c r="G53" s="43" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="54" spans="1:8" s="28" customFormat="1">
@@ -10929,24 +11008,24 @@
       <c r="C54" s="146" t="s">
         <v>54</v>
       </c>
-      <c r="E54" s="158" t="s">
+      <c r="E54" s="156" t="s">
         <v>262</v>
       </c>
-      <c r="F54" s="158"/>
+      <c r="F54" s="156"/>
       <c r="G54" s="7" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="55" spans="1:8" s="28" customFormat="1" ht="31.5">
       <c r="A55" s="20"/>
       <c r="B55" s="20"/>
       <c r="C55" s="20"/>
-      <c r="E55" s="158" t="s">
+      <c r="E55" s="156" t="s">
         <v>262</v>
       </c>
-      <c r="F55" s="158"/>
+      <c r="F55" s="156"/>
       <c r="G55" s="130" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="56" spans="1:8" s="28" customFormat="1">
@@ -11183,7 +11262,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K94"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -11217,11 +11296,11 @@
       <c r="B2" s="25">
         <v>43279</v>
       </c>
-      <c r="C2" s="156" t="s">
-        <v>683</v>
-      </c>
-      <c r="D2" s="157"/>
-      <c r="E2" s="157"/>
+      <c r="C2" s="157" t="s">
+        <v>682</v>
+      </c>
+      <c r="D2" s="158"/>
+      <c r="E2" s="158"/>
       <c r="G2" s="41" t="s">
         <v>195</v>
       </c>
@@ -11231,9 +11310,9 @@
         <v>46</v>
       </c>
       <c r="B3" s="145"/>
-      <c r="C3" s="157"/>
-      <c r="D3" s="157"/>
-      <c r="E3" s="157"/>
+      <c r="C3" s="158"/>
+      <c r="D3" s="158"/>
+      <c r="E3" s="158"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="10" t="s">
@@ -11242,16 +11321,16 @@
       <c r="B4" s="145" t="s">
         <v>367</v>
       </c>
-      <c r="C4" s="157"/>
-      <c r="D4" s="157"/>
-      <c r="E4" s="157"/>
+      <c r="C4" s="158"/>
+      <c r="D4" s="158"/>
+      <c r="E4" s="158"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="20"/>
       <c r="B5" s="145"/>
-      <c r="C5" s="157"/>
-      <c r="D5" s="157"/>
-      <c r="E5" s="157"/>
+      <c r="C5" s="158"/>
+      <c r="D5" s="158"/>
+      <c r="E5" s="158"/>
     </row>
     <row r="6" spans="1:11" s="9" customFormat="1" ht="47.25">
       <c r="A6" s="39" t="s">
@@ -11384,7 +11463,7 @@
         <v>199</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="C12" s="45" t="s">
         <v>547</v>
@@ -11396,7 +11475,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="43" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="H12" s="58"/>
       <c r="I12" s="58"/>
@@ -11599,7 +11678,7 @@
         <v>2</v>
       </c>
       <c r="G22" s="97" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -11607,7 +11686,7 @@
         <v>199</v>
       </c>
       <c r="B23" s="130" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="C23" s="129" t="s">
         <v>554</v>
@@ -11619,7 +11698,7 @@
         <v>3</v>
       </c>
       <c r="G23" s="97" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -11640,7 +11719,7 @@
         <v>4</v>
       </c>
       <c r="G24" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="25" spans="1:11" s="28" customFormat="1" ht="31.5">
@@ -11660,7 +11739,7 @@
         <v>5</v>
       </c>
       <c r="G25" s="28" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="26" spans="1:11" s="28" customFormat="1">
@@ -11794,7 +11873,7 @@
         <v>564</v>
       </c>
       <c r="C34" s="129" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>189</v>
@@ -11803,7 +11882,7 @@
         <v>3</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="43" customFormat="1" ht="31.5">
@@ -11814,7 +11893,7 @@
         <v>643</v>
       </c>
       <c r="C35" s="129" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="E35" s="7" t="s">
         <v>189</v>
@@ -11831,7 +11910,7 @@
         <v>644</v>
       </c>
       <c r="C36" s="129" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>189</v>
@@ -11848,7 +11927,7 @@
         <v>645</v>
       </c>
       <c r="C37" s="129" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>189</v>
@@ -11920,12 +11999,12 @@
       <c r="C42" s="148" t="s">
         <v>500</v>
       </c>
-      <c r="E42" s="158" t="s">
+      <c r="E42" s="156" t="s">
         <v>262</v>
       </c>
-      <c r="F42" s="158"/>
+      <c r="F42" s="156"/>
       <c r="G42" s="44" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="43" customFormat="1" ht="47.25">
@@ -11936,12 +12015,12 @@
       <c r="C43" s="148" t="s">
         <v>566</v>
       </c>
-      <c r="E43" s="158" t="s">
+      <c r="E43" s="156" t="s">
         <v>262</v>
       </c>
-      <c r="F43" s="158"/>
+      <c r="F43" s="156"/>
       <c r="G43" s="44" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="43" customFormat="1" ht="63">
@@ -11952,12 +12031,12 @@
       <c r="C44" s="148" t="s">
         <v>145</v>
       </c>
-      <c r="E44" s="158" t="s">
+      <c r="E44" s="156" t="s">
         <v>262</v>
       </c>
-      <c r="F44" s="158"/>
+      <c r="F44" s="156"/>
       <c r="G44" s="130" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="H44" s="44" t="s">
         <v>418</v>
@@ -11968,7 +12047,7 @@
         <v>229</v>
       </c>
       <c r="B45" s="49" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="C45" s="53" t="s">
         <v>189</v>
@@ -12005,7 +12084,7 @@
         <v>1</v>
       </c>
       <c r="G46" s="44" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="47" spans="1:9" s="43" customFormat="1">
@@ -12042,7 +12121,7 @@
         <v>3</v>
       </c>
       <c r="G48" s="43" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="49" spans="1:8" s="43" customFormat="1" ht="35.25" customHeight="1">
@@ -12090,12 +12169,12 @@
       <c r="C51" s="148" t="s">
         <v>54</v>
       </c>
-      <c r="E51" s="158" t="s">
+      <c r="E51" s="156" t="s">
         <v>262</v>
       </c>
-      <c r="F51" s="158"/>
+      <c r="F51" s="156"/>
       <c r="G51" s="130" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="52" spans="1:8" s="28" customFormat="1">
@@ -12333,8 +12412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K95"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -12365,13 +12444,13 @@
         <v>45</v>
       </c>
       <c r="B2" s="25">
-        <v>43279</v>
-      </c>
-      <c r="C2" s="156" t="s">
-        <v>683</v>
-      </c>
-      <c r="D2" s="157"/>
-      <c r="E2" s="157"/>
+        <v>43292</v>
+      </c>
+      <c r="C2" s="157" t="s">
+        <v>797</v>
+      </c>
+      <c r="D2" s="158"/>
+      <c r="E2" s="158"/>
       <c r="G2" s="41" t="s">
         <v>195</v>
       </c>
@@ -12381,9 +12460,9 @@
         <v>46</v>
       </c>
       <c r="B3" s="145"/>
-      <c r="C3" s="157"/>
-      <c r="D3" s="157"/>
-      <c r="E3" s="157"/>
+      <c r="C3" s="158"/>
+      <c r="D3" s="158"/>
+      <c r="E3" s="158"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="10" t="s">
@@ -12392,16 +12471,16 @@
       <c r="B4" s="145" t="s">
         <v>367</v>
       </c>
-      <c r="C4" s="157"/>
-      <c r="D4" s="157"/>
-      <c r="E4" s="157"/>
+      <c r="C4" s="158"/>
+      <c r="D4" s="158"/>
+      <c r="E4" s="158"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="20"/>
       <c r="B5" s="145"/>
-      <c r="C5" s="157"/>
-      <c r="D5" s="157"/>
-      <c r="E5" s="157"/>
+      <c r="C5" s="158"/>
+      <c r="D5" s="158"/>
+      <c r="E5" s="158"/>
     </row>
     <row r="6" spans="1:11" s="9" customFormat="1" ht="47.25">
       <c r="A6" s="39" t="s">
@@ -12512,7 +12591,7 @@
         <v>199</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>372</v>
@@ -12524,7 +12603,7 @@
         <v>2</v>
       </c>
       <c r="G11" s="43" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="H11" s="58"/>
       <c r="I11" s="58"/>
@@ -12536,7 +12615,7 @@
         <v>199</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>372</v>
@@ -12580,7 +12659,7 @@
         <v>199</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>302</v>
@@ -12777,7 +12856,7 @@
         <v>4</v>
       </c>
       <c r="G24" s="44" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="25" spans="1:11" s="98" customFormat="1" ht="31.5">
@@ -12785,7 +12864,7 @@
         <v>199</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>363</v>
@@ -12892,7 +12971,7 @@
       </c>
       <c r="F32" s="155"/>
       <c r="G32" s="130" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="H32" s="13" t="s">
         <v>378</v>
@@ -12993,7 +13072,7 @@
         <v>4</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="H37" s="44"/>
     </row>
@@ -13032,7 +13111,7 @@
         <v>6</v>
       </c>
       <c r="G39" s="43" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="H39" s="13" t="s">
         <v>420</v>
@@ -13097,7 +13176,7 @@
         <v>229</v>
       </c>
       <c r="B44" s="49" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="C44" s="53" t="s">
         <v>189</v>
@@ -13229,7 +13308,7 @@
       </c>
       <c r="F50" s="159"/>
       <c r="G50" s="119" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="H50" s="44" t="s">
         <v>419</v>
@@ -13249,7 +13328,7 @@
       </c>
       <c r="F51" s="159"/>
       <c r="G51" s="119" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="H51" s="44" t="s">
         <v>421</v>
@@ -13543,8 +13622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K98"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -13575,13 +13654,13 @@
         <v>45</v>
       </c>
       <c r="B2" s="25">
-        <v>43279</v>
-      </c>
-      <c r="C2" s="156" t="s">
-        <v>683</v>
-      </c>
-      <c r="D2" s="157"/>
-      <c r="E2" s="157"/>
+        <v>43292</v>
+      </c>
+      <c r="C2" s="157" t="s">
+        <v>797</v>
+      </c>
+      <c r="D2" s="158"/>
+      <c r="E2" s="158"/>
       <c r="G2" s="41" t="s">
         <v>195</v>
       </c>
@@ -13590,10 +13669,10 @@
       <c r="A3" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="145"/>
-      <c r="C3" s="157"/>
-      <c r="D3" s="157"/>
-      <c r="E3" s="157"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="158"/>
+      <c r="D3" s="158"/>
+      <c r="E3" s="158"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="10" t="s">
@@ -13602,16 +13681,16 @@
       <c r="B4" s="145" t="s">
         <v>367</v>
       </c>
-      <c r="C4" s="157"/>
-      <c r="D4" s="157"/>
-      <c r="E4" s="157"/>
+      <c r="C4" s="158"/>
+      <c r="D4" s="158"/>
+      <c r="E4" s="158"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="20"/>
       <c r="B5" s="145"/>
-      <c r="C5" s="157"/>
-      <c r="D5" s="157"/>
-      <c r="E5" s="157"/>
+      <c r="C5" s="158"/>
+      <c r="D5" s="158"/>
+      <c r="E5" s="158"/>
     </row>
     <row r="6" spans="1:11" s="9" customFormat="1" ht="47.25">
       <c r="A6" s="39" t="s">
@@ -13676,7 +13755,7 @@
         <v>198</v>
       </c>
       <c r="B9" s="48" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="C9" s="53" t="s">
         <v>189</v>
@@ -13700,7 +13779,7 @@
         <v>199</v>
       </c>
       <c r="B10" s="68" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="C10" s="45" t="s">
         <v>441</v>
@@ -13741,7 +13820,7 @@
         <v>199</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="C12" s="45" t="s">
         <v>442</v>
@@ -13753,7 +13832,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="58" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="H12" s="58"/>
       <c r="I12" s="58"/>
@@ -13765,7 +13844,7 @@
         <v>199</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
       <c r="C13" s="45" t="s">
         <v>353</v>
@@ -13809,7 +13888,7 @@
         <v>199</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="C15" s="93" t="s">
         <v>451</v>
@@ -13831,7 +13910,7 @@
         <v>199</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="E16" s="59" t="s">
         <v>212</v>
@@ -13850,7 +13929,7 @@
         <v>199</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="E17" s="59" t="s">
         <v>212</v>
@@ -13869,7 +13948,7 @@
         <v>199</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="E18" s="43" t="s">
         <v>212</v>
@@ -13911,7 +13990,7 @@
       <c r="E20" s="43"/>
       <c r="F20" s="59"/>
       <c r="G20" s="58" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="H20" s="58"/>
       <c r="I20" s="58"/>
@@ -13972,7 +14051,7 @@
         <v>199</v>
       </c>
       <c r="B23" s="77" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="C23" s="77" t="s">
         <v>447</v>
@@ -13984,7 +14063,7 @@
         <v>1</v>
       </c>
       <c r="G23" s="91" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="H23" s="110" t="s">
         <v>465</v>
@@ -13995,7 +14074,7 @@
         <v>199</v>
       </c>
       <c r="B24" s="112" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
       <c r="C24" s="105" t="s">
         <v>448</v>
@@ -14018,7 +14097,7 @@
         <v>199</v>
       </c>
       <c r="B25" s="150" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="C25" s="77" t="s">
         <v>448</v>
@@ -14030,7 +14109,7 @@
         <v>3</v>
       </c>
       <c r="G25" s="91" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="H25" s="110" t="s">
         <v>422</v>
@@ -14145,7 +14224,7 @@
         <v>198</v>
       </c>
       <c r="B34" s="49" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="C34" s="53" t="s">
         <v>189</v>
@@ -14170,7 +14249,7 @@
         <v>199</v>
       </c>
       <c r="B35" s="152" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="C35" s="152" t="s">
         <v>451</v>
@@ -14182,7 +14261,7 @@
         <v>1</v>
       </c>
       <c r="G35" s="43" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
     </row>
     <row r="36" spans="1:9" s="43" customFormat="1" ht="47.25">
@@ -14190,7 +14269,7 @@
         <v>199</v>
       </c>
       <c r="B36" s="152" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="C36" s="152" t="s">
         <v>459</v>
@@ -14202,7 +14281,7 @@
         <v>2</v>
       </c>
       <c r="G36" s="43" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="H36" s="110" t="s">
         <v>422</v>
@@ -14225,7 +14304,7 @@
         <v>3</v>
       </c>
       <c r="G37" s="43" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
     </row>
     <row r="38" spans="1:9" s="43" customFormat="1" ht="31.5">
@@ -14233,7 +14312,7 @@
         <v>199</v>
       </c>
       <c r="B38" s="152" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="C38" s="152" t="s">
         <v>460</v>
@@ -14245,7 +14324,7 @@
         <v>4</v>
       </c>
       <c r="G38" s="43" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="H38" s="110" t="s">
         <v>422</v>
@@ -14268,7 +14347,7 @@
         <v>5</v>
       </c>
       <c r="G39" s="43" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="H39" s="43" t="s">
         <v>462</v>
@@ -14343,10 +14422,10 @@
       <c r="C45" s="152" t="s">
         <v>453</v>
       </c>
-      <c r="E45" s="158" t="s">
+      <c r="E45" s="156" t="s">
         <v>262</v>
       </c>
-      <c r="F45" s="158"/>
+      <c r="F45" s="156"/>
       <c r="G45" s="43" t="s">
         <v>469</v>
       </c>
@@ -14362,10 +14441,10 @@
       <c r="C46" s="152" t="s">
         <v>455</v>
       </c>
-      <c r="E46" s="158" t="s">
+      <c r="E46" s="156" t="s">
         <v>262</v>
       </c>
-      <c r="F46" s="158"/>
+      <c r="F46" s="156"/>
       <c r="G46" s="43" t="s">
         <v>469</v>
       </c>
@@ -14381,12 +14460,12 @@
       <c r="C47" s="152" t="s">
         <v>456</v>
       </c>
-      <c r="E47" s="158" t="s">
+      <c r="E47" s="156" t="s">
         <v>262</v>
       </c>
-      <c r="F47" s="158"/>
+      <c r="F47" s="156"/>
       <c r="G47" s="130" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="H47" s="58" t="s">
         <v>463</v>
@@ -14397,7 +14476,7 @@
         <v>229</v>
       </c>
       <c r="B48" s="49" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="C48" s="53" t="s">
         <v>189</v>
@@ -14512,12 +14591,12 @@
       <c r="C54" s="152" t="s">
         <v>54</v>
       </c>
-      <c r="E54" s="158" t="s">
+      <c r="E54" s="156" t="s">
         <v>262</v>
       </c>
-      <c r="F54" s="158"/>
+      <c r="F54" s="156"/>
       <c r="G54" s="130" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="H54" s="110" t="s">
         <v>422</v>
@@ -14765,8 +14844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K93"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -14798,13 +14877,13 @@
         <v>45</v>
       </c>
       <c r="B2" s="25">
-        <v>43279</v>
-      </c>
-      <c r="C2" s="156" t="s">
-        <v>683</v>
-      </c>
-      <c r="D2" s="157"/>
-      <c r="E2" s="157"/>
+        <v>43292</v>
+      </c>
+      <c r="C2" s="157" t="s">
+        <v>797</v>
+      </c>
+      <c r="D2" s="158"/>
+      <c r="E2" s="158"/>
       <c r="G2" s="41" t="s">
         <v>195</v>
       </c>
@@ -14814,9 +14893,9 @@
         <v>46</v>
       </c>
       <c r="B3" s="145"/>
-      <c r="C3" s="157"/>
-      <c r="D3" s="157"/>
-      <c r="E3" s="157"/>
+      <c r="C3" s="158"/>
+      <c r="D3" s="158"/>
+      <c r="E3" s="158"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="88" t="s">
@@ -14825,16 +14904,16 @@
       <c r="B4" s="145" t="s">
         <v>367</v>
       </c>
-      <c r="C4" s="157"/>
-      <c r="D4" s="157"/>
-      <c r="E4" s="157"/>
+      <c r="C4" s="158"/>
+      <c r="D4" s="158"/>
+      <c r="E4" s="158"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="87"/>
       <c r="B5" s="145"/>
-      <c r="C5" s="157"/>
-      <c r="D5" s="157"/>
-      <c r="E5" s="157"/>
+      <c r="C5" s="158"/>
+      <c r="D5" s="158"/>
+      <c r="E5" s="158"/>
     </row>
     <row r="6" spans="1:11" s="9" customFormat="1" ht="47.25">
       <c r="A6" s="39" t="s">
@@ -14923,7 +15002,7 @@
         <v>199</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
       <c r="C10" s="45" t="s">
         <v>408</v>
@@ -14979,7 +15058,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="43" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="H12" s="58"/>
       <c r="I12" s="58"/>
@@ -15135,10 +15214,10 @@
         <v>199</v>
       </c>
       <c r="B21" s="77" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C21" s="116" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="E21" s="59">
         <v>1</v>
@@ -15147,7 +15226,7 @@
         <v>1</v>
       </c>
       <c r="G21" s="106" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -15175,7 +15254,7 @@
         <v>199</v>
       </c>
       <c r="B23" s="77" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="C23" s="94" t="s">
         <v>417</v>
@@ -15195,10 +15274,10 @@
         <v>199</v>
       </c>
       <c r="B24" s="109" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="C24" s="119" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E24" s="59">
         <v>4</v>
@@ -15207,7 +15286,7 @@
         <v>4</v>
       </c>
       <c r="G24" s="97" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="25" spans="1:11" s="100" customFormat="1">
@@ -15296,7 +15375,7 @@
       </c>
       <c r="F31" s="155"/>
       <c r="G31" s="45" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="H31" s="103" t="s">
         <v>404</v>
@@ -15315,7 +15394,7 @@
       </c>
       <c r="F32" s="155"/>
       <c r="G32" s="130" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="H32" s="108" t="s">
         <v>418</v>
@@ -15603,7 +15682,7 @@
       </c>
       <c r="F50" s="155"/>
       <c r="G50" s="130" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="51" spans="1:8" s="100" customFormat="1">
@@ -15854,8 +15933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -15888,10 +15967,10 @@
         <v>45</v>
       </c>
       <c r="B2" s="31">
-        <v>43279</v>
+        <v>43292</v>
       </c>
       <c r="C2" s="154" t="s">
-        <v>749</v>
+        <v>798</v>
       </c>
       <c r="D2" s="154"/>
       <c r="E2" s="154"/>
@@ -16007,10 +16086,10 @@
         <v>199</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="E10" s="65">
         <v>1</v>
@@ -16075,7 +16154,7 @@
         <v>199</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>313</v>
@@ -16087,7 +16166,7 @@
         <v>5</v>
       </c>
       <c r="G14" s="136" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="H14" s="7" t="s">
         <v>596</v>
@@ -16252,7 +16331,7 @@
         <v>199</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="C25" s="64"/>
       <c r="E25" s="65">
@@ -16262,7 +16341,7 @@
         <v>4</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="H25" s="7"/>
     </row>
@@ -16406,7 +16485,7 @@
         <v>199</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="C35" s="128" t="s">
         <v>316</v>
@@ -16418,7 +16497,7 @@
         <v>3</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="H35" s="65"/>
     </row>
@@ -16427,7 +16506,7 @@
         <v>199</v>
       </c>
       <c r="B36" s="112" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="E36" s="65" t="s">
         <v>189</v>
@@ -16436,17 +16515,17 @@
         <v>4</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="H36" s="65"/>
     </row>
     <row r="37" spans="1:8" ht="47.25">
       <c r="A37" s="73"/>
       <c r="B37" s="130" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="C37" s="112" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="E37" s="65" t="s">
         <v>189</v>
@@ -16455,7 +16534,7 @@
         <v>5</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="H37" s="130" t="s">
         <v>590</v>
@@ -16686,7 +16765,7 @@
       </c>
       <c r="F50" s="159"/>
       <c r="G50" s="130" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="52" spans="1:7">

</xml_diff>